<commit_message>
Further updates to tidy up code before publication
</commit_message>
<xml_diff>
--- a/CipherSuiteTestResults.xlsx
+++ b/CipherSuiteTestResults.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy\Projects\SecurityTest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andy\Projects\FSDemoApp\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -523,60 +523,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -864,8 +815,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>